<commit_message>
working on battle & optimize exporter
</commit_message>
<xml_diff>
--- a/plan/excel/aura_光环表.xlsx
+++ b/plan/excel/aura_光环表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="AuraProto" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -33,7 +33,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -196,10 +196,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>duration</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>n</t>
     </r>
@@ -217,10 +213,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>uptime</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>number</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -286,6 +278,14 @@
   </si>
   <si>
     <t>这个光环真有用</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>last_t</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>itv_t</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -391,7 +391,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -681,17 +681,17 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="7.453125" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.90625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -708,25 +708,25 @@
         <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -755,13 +755,13 @@
         <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -772,31 +772,31 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -807,31 +807,31 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -863,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -898,10 +898,10 @@
         <v>0</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2001</v>
       </c>
@@ -933,10 +933,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -968,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -1003,10 +1003,10 @@
         <v>0</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -1038,10 +1038,10 @@
         <v>0</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -1073,10 +1073,10 @@
         <v>0</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -1108,10 +1108,10 @@
         <v>0</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1143,10 +1143,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -1178,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -1213,10 +1213,10 @@
         <v>0</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1248,10 +1248,10 @@
         <v>0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -1283,10 +1283,10 @@
         <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -1318,10 +1318,10 @@
         <v>0</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* new skill & aura
</commit_message>
<xml_diff>
--- a/plan/excel/aura_光环表.xlsx
+++ b/plan/excel/aura_光环表.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -205,14 +205,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>脚本ID</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>参数1</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -377,6 +369,55 @@
   <si>
     <t>9秒内减少6次伤害，每次减少30点</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血光环</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>none</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血10%造成的伤害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血20%造成的伤害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血30%造成的伤害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血40%造成的伤害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>吸血50%造成的伤害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>掉防光环</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>掉7点防御</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>掉11点防御</t>
+  </si>
+  <si>
+    <t>掉9点防御</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>掉13点防御</t>
+  </si>
+  <si>
+    <t>掉15点防御</t>
   </si>
 </sst>
 </file>
@@ -767,21 +808,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.75" customWidth="1"/>
+    <col min="12" max="12" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -798,31 +839,28 @@
         <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -839,10 +877,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -854,16 +892,13 @@
         <v>13</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -874,37 +909,34 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -921,10 +953,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>15</v>
@@ -939,13 +971,10 @@
         <v>15</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -953,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>3000</v>
@@ -962,16 +991,16 @@
         <v>1000</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -979,14 +1008,11 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -994,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>4000</v>
@@ -1003,16 +1029,16 @@
         <v>1000</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I6">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1020,14 +1046,11 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2001</v>
       </c>
@@ -1035,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>5000</v>
@@ -1044,16 +1067,16 @@
         <v>1000</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="I7">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1061,14 +1084,11 @@
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1076,7 +1096,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>6000</v>
@@ -1085,16 +1105,16 @@
         <v>1000</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="I8">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1102,14 +1122,11 @@
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -1117,7 +1134,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>7000</v>
@@ -1126,16 +1143,16 @@
         <v>1000</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="I9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1143,14 +1160,11 @@
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -1158,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>4500</v>
@@ -1167,16 +1181,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1184,14 +1198,11 @@
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L10" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -1199,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>4500</v>
@@ -1208,16 +1219,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1225,14 +1236,11 @@
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -1240,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>4500</v>
@@ -1249,16 +1257,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="I12">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1266,14 +1274,11 @@
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L12" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1281,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>4500</v>
@@ -1290,31 +1295,28 @@
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -1322,7 +1324,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>4500</v>
@@ -1331,16 +1333,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14">
         <v>50</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
       <c r="I14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1348,14 +1350,11 @@
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>5000</v>
@@ -1372,31 +1371,28 @@
         <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>10</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1404,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>6000</v>
@@ -1413,31 +1409,28 @@
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H16">
         <v>3</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J16">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -1445,7 +1438,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>7000</v>
@@ -1454,31 +1447,28 @@
         <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L17" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -1486,7 +1476,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>8000</v>
@@ -1495,31 +1485,28 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I18">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="J18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="L18" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -1527,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>9000</v>
@@ -1536,28 +1523,405 @@
         <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2004</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <v>4000</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2004</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>4000</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>2004</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22">
+        <v>4000</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22">
+        <v>30</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>2004</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>4000</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23">
+        <v>40</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>2004</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24">
+        <v>4000</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24">
         <v>50</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>2005</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25">
+        <v>3000</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25">
+        <v>7</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>2005</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26">
+        <v>3000</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26">
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>2005</v>
+      </c>
+      <c r="B27">
         <v>3</v>
       </c>
-      <c r="I19">
-        <v>6</v>
-      </c>
-      <c r="J19">
-        <v>30</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27">
+        <v>3000</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>2005</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28">
+        <v>3000</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28">
+        <v>13</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>2005</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29">
+        <v>3000</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29">
+        <v>15</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* new excel format
</commit_message>
<xml_diff>
--- a/plan/excel/aura_光环表.xlsx
+++ b/plan/excel/aura_光环表.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="AuraProto" sheetId="4" r:id="rId1"/>
+    <sheet name="脚本ID说明" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AuraProto!$A$1:$C$4</definedName>
@@ -19,7 +20,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -33,7 +34,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -73,6 +74,63 @@
           <t xml:space="preserve">
 单位：毫秒
 0：无间隔时间</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>详情见</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>sheet</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>脚本</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ID</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>说明</t>
         </r>
       </text>
     </comment>
@@ -100,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="73">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -419,12 +477,32 @@
     <t>光环名字</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>array</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>脚本ID</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>script_id</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +552,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -506,7 +591,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -522,7 +607,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -808,21 +893,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.75" customWidth="1"/>
+    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="13" max="13" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -845,22 +931,25 @@
         <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -883,7 +972,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
@@ -892,13 +981,16 @@
         <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -921,22 +1013,25 @@
         <v>45</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -959,7 +1054,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>13</v>
@@ -968,13 +1063,16 @@
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -996,23 +1094,23 @@
       <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>20</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -1034,23 +1132,23 @@
       <c r="G6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>40</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2001</v>
       </c>
@@ -1072,23 +1170,23 @@
       <c r="G7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>60</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1110,23 +1208,23 @@
       <c r="G8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>80</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -1148,23 +1246,23 @@
       <c r="G9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>100</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -1186,23 +1284,23 @@
       <c r="G10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10">
         <v>10</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -1224,23 +1322,23 @@
       <c r="G11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
+      <c r="I11">
         <v>20</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -1262,23 +1360,23 @@
       <c r="G12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12">
         <v>30</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1300,23 +1398,23 @@
       <c r="G13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>40</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -1338,23 +1436,23 @@
       <c r="G14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <v>50</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -1376,23 +1474,23 @@
       <c r="G15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15">
         <v>2</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>10</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1414,23 +1512,23 @@
       <c r="G16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>3</v>
       </c>
       <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
         <v>15</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -1452,23 +1550,23 @@
       <c r="G17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17">
         <v>4</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>20</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -1490,23 +1588,23 @@
       <c r="G18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+      <c r="I18">
         <v>5</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>25</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -1528,23 +1626,23 @@
       <c r="G19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
+        <v>3</v>
+      </c>
+      <c r="I19">
         <v>6</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>30</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2004</v>
       </c>
@@ -1566,23 +1664,23 @@
       <c r="G20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
+        <v>4</v>
+      </c>
+      <c r="I20">
         <v>10</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -1604,23 +1702,23 @@
       <c r="G21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
+        <v>4</v>
+      </c>
+      <c r="I21">
         <v>20</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1642,23 +1740,23 @@
       <c r="G22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="3">
+        <v>4</v>
+      </c>
+      <c r="I22">
         <v>30</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2004</v>
       </c>
@@ -1680,23 +1778,23 @@
       <c r="G23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
+        <v>4</v>
+      </c>
+      <c r="I23">
         <v>40</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>2004</v>
       </c>
@@ -1718,23 +1816,23 @@
       <c r="G24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="3">
+        <v>4</v>
+      </c>
+      <c r="I24">
         <v>50</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>2005</v>
       </c>
@@ -1756,23 +1854,23 @@
       <c r="G25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="3">
+        <v>5</v>
+      </c>
+      <c r="I25">
         <v>7</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>2005</v>
       </c>
@@ -1794,23 +1892,23 @@
       <c r="G26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
+        <v>5</v>
+      </c>
+      <c r="I26">
         <v>9</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -1832,23 +1930,23 @@
       <c r="G27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="3">
+        <v>5</v>
+      </c>
+      <c r="I27">
         <v>11</v>
       </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
       <c r="J27">
         <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>2005</v>
       </c>
@@ -1870,23 +1968,23 @@
       <c r="G28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="3">
+        <v>5</v>
+      </c>
+      <c r="I28">
         <v>13</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
       <c r="J28">
         <v>0</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>2005</v>
       </c>
@@ -1908,19 +2006,19 @@
       <c r="G29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="3">
+        <v>5</v>
+      </c>
+      <c r="I29">
         <v>15</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
       <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1930,4 +2028,17 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add icon on excel
</commit_message>
<xml_diff>
--- a/plan/excel/aura_光环表.xlsx
+++ b/plan/excel/aura_光环表.xlsx
@@ -77,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="82">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -496,6 +496,37 @@
   <si>
     <t>number</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICON</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>l</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon/aura/aura_2001.png</t>
+  </si>
+  <si>
+    <t>icon/aura/aura_2002.png</t>
+  </si>
+  <si>
+    <t>icon/aura/aura_2003.png</t>
+  </si>
+  <si>
+    <t>icon/aura/aura_2004.png</t>
+  </si>
+  <si>
+    <t>icon/aura/aura_2005.png</t>
   </si>
 </sst>
 </file>
@@ -893,22 +924,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
-    <col min="13" max="13" width="37.75" customWidth="1"/>
+    <col min="8" max="8" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="14" max="14" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -931,25 +963,28 @@
         <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -972,10 +1007,10 @@
         <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
@@ -984,13 +1019,16 @@
         <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1013,25 +1051,28 @@
         <v>45</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1054,25 +1095,28 @@
         <v>26</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -1094,23 +1138,26 @@
       <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>20</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -1132,23 +1179,26 @@
       <c r="G6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="3">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>40</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2001</v>
       </c>
@@ -1170,23 +1220,26 @@
       <c r="G7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>60</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1208,23 +1261,26 @@
       <c r="G8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="3">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>80</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -1246,23 +1302,26 @@
       <c r="G9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>100</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -1284,23 +1343,26 @@
       <c r="G10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="3">
         <v>2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>10</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -1322,23 +1384,26 @@
       <c r="G11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="3">
         <v>2</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>20</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
       <c r="K11">
         <v>0</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -1360,23 +1425,26 @@
       <c r="G12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="3">
         <v>2</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>30</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1398,23 +1466,26 @@
       <c r="G13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="3">
         <v>2</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>40</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -1436,23 +1507,26 @@
       <c r="G14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="3">
         <v>2</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>50</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="K14">
         <v>0</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -1474,23 +1548,26 @@
       <c r="G15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="3">
         <v>3</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>10</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1512,23 +1589,26 @@
       <c r="G16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="3">
         <v>3</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>3</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>15</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="3" t="s">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -1550,23 +1630,26 @@
       <c r="G17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="3">
         <v>3</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>4</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>20</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3" t="s">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -1588,23 +1671,26 @@
       <c r="G18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="3">
         <v>3</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>5</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>25</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3" t="s">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -1626,23 +1712,26 @@
       <c r="G19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="3">
         <v>3</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>6</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>30</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="3" t="s">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="N19" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2004</v>
       </c>
@@ -1664,23 +1753,26 @@
       <c r="G20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="3">
         <v>4</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>10</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -1702,23 +1794,26 @@
       <c r="G21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="3">
         <v>4</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>20</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="N21" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1740,23 +1835,26 @@
       <c r="G22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="3">
         <v>4</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>30</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2004</v>
       </c>
@@ -1778,23 +1876,26 @@
       <c r="G23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="3">
         <v>4</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>40</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="N23" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>2004</v>
       </c>
@@ -1816,23 +1917,26 @@
       <c r="G24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" s="3">
         <v>4</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>50</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
       <c r="K24">
         <v>0</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>2005</v>
       </c>
@@ -1854,23 +1958,26 @@
       <c r="G25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="3">
         <v>5</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>7</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>2005</v>
       </c>
@@ -1892,23 +1999,26 @@
       <c r="G26" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="3">
         <v>5</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>9</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
       <c r="K26">
         <v>0</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -1930,23 +2040,26 @@
       <c r="G27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="3">
         <v>5</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>11</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>2005</v>
       </c>
@@ -1968,23 +2081,26 @@
       <c r="G28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="3">
         <v>5</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>13</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>2005</v>
       </c>
@@ -2006,19 +2122,22 @@
       <c r="G29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="3">
         <v>5</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>15</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on battle fix
</commit_message>
<xml_diff>
--- a/plan/excel/aura_光环表.xlsx
+++ b/plan/excel/aura_光环表.xlsx
@@ -77,7 +77,63 @@
         </r>
       </text>
     </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+0:不可被删除
+1:可被删除</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+对owner有益与否
+0:不计较
+1:有益
+2:有害</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
   <si>
     <t>number</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -255,42 +311,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>参数1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>参数2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>参数3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>参数4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>jl</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>param1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>param2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>param3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>param4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>描述</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -336,10 +356,6 @@
   </si>
   <si>
     <t>每秒回复100点HP</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>增加10点攻击</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -486,6 +502,228 @@
   </si>
   <si>
     <t>icon/aura/aura_2005.png</t>
+  </si>
+  <si>
+    <t>是否有益</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>helpful</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>j</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>props#id_part_val</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>params</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|10</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|15</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|20</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|25</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|30</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加10基础点攻击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_0_50</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_0_10</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_0_20</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_0_30</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_0_40</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_2_-7</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_2_-9</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_2_-11</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_2_-13</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_2_-15</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>脚本I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能描述</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>每次update恢复HP</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始、结束时分别增加、减少属性</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>光环时间段时，抵挡x次伤害</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>给敌人造成伤害时，吸血</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>deletable</t>
+  </si>
+  <si>
+    <t>可否被清除</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -887,27 +1125,29 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
+    <col min="8" max="8" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="23.625" customWidth="1"/>
     <col min="12" max="12" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -916,25 +1156,25 @@
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
@@ -951,28 +1191,28 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -986,31 +1226,31 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1027,28 +1267,28 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1059,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>3000</v>
@@ -1067,23 +1307,24 @@
       <c r="E5">
         <v>1000</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5">
         <v>20</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="L5" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
@@ -1094,7 +1335,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>4000</v>
@@ -1102,23 +1343,24 @@
       <c r="E6">
         <v>1000</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6">
         <v>40</v>
       </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -1129,7 +1371,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>5000</v>
@@ -1137,23 +1379,24 @@
       <c r="E7">
         <v>1000</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7">
+        <v>60</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
@@ -1164,7 +1407,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>6000</v>
@@ -1172,23 +1415,24 @@
       <c r="E8">
         <v>1000</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8">
         <v>80</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="L8" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
@@ -1199,7 +1443,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>7000</v>
@@ -1207,23 +1451,24 @@
       <c r="E9">
         <v>1000</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9">
         <v>100</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="L9" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
@@ -1234,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>4500</v>
@@ -1242,23 +1487,26 @@
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="3">
         <v>2</v>
       </c>
-      <c r="H10">
+      <c r="J10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10">
         <v>10</v>
       </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
@@ -1269,7 +1517,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>4500</v>
@@ -1277,23 +1525,26 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="3">
         <v>2</v>
       </c>
-      <c r="H11">
+      <c r="J11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11">
         <v>20</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
       <c r="L11" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -1304,7 +1555,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>4500</v>
@@ -1312,23 +1563,26 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="3">
         <v>2</v>
       </c>
-      <c r="H12">
+      <c r="J12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12">
         <v>30</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -1339,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>4500</v>
@@ -1347,23 +1601,26 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="3">
         <v>2</v>
       </c>
-      <c r="H13">
+      <c r="J13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13">
         <v>40</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="L13" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -1374,7 +1631,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>4500</v>
@@ -1382,23 +1639,26 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="3">
         <v>2</v>
       </c>
-      <c r="H14">
+      <c r="J14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14">
         <v>50</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="L14" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -1409,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>5000</v>
@@ -1417,23 +1677,24 @@
       <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="3">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>10</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="L15" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
@@ -1444,7 +1705,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D16">
         <v>6000</v>
@@ -1452,23 +1713,24 @@
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="3">
         <v>3</v>
       </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16">
-        <v>15</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
@@ -1479,7 +1741,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>7000</v>
@@ -1487,23 +1749,24 @@
       <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="3">
         <v>3</v>
       </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <v>20</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.15">
@@ -1514,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>8000</v>
@@ -1522,23 +1785,24 @@
       <c r="E18">
         <v>0</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="3">
         <v>3</v>
       </c>
-      <c r="H18">
-        <v>5</v>
-      </c>
-      <c r="I18">
-        <v>25</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
@@ -1549,7 +1813,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D19">
         <v>9000</v>
@@ -1557,23 +1821,24 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="3">
         <v>3</v>
       </c>
-      <c r="H19">
-        <v>6</v>
-      </c>
-      <c r="I19">
-        <v>30</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
@@ -1584,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>4000</v>
@@ -1592,23 +1857,24 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="3">
         <v>4</v>
       </c>
-      <c r="H20">
+      <c r="J20" s="3"/>
+      <c r="K20">
         <v>10</v>
       </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="L20" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
@@ -1619,7 +1885,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>4000</v>
@@ -1627,23 +1893,24 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="3">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="3">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="J21" s="3"/>
+      <c r="K21">
         <v>20</v>
       </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
       <c r="L21" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
@@ -1654,7 +1921,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D22">
         <v>4000</v>
@@ -1662,23 +1929,24 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="3">
         <v>4</v>
       </c>
-      <c r="H22">
+      <c r="J22" s="3"/>
+      <c r="K22">
         <v>30</v>
       </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
       <c r="L22" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.15">
@@ -1689,7 +1957,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>4000</v>
@@ -1697,23 +1965,24 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" s="3">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="3">
         <v>4</v>
       </c>
-      <c r="H23">
+      <c r="J23" s="3"/>
+      <c r="K23">
         <v>40</v>
       </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
       <c r="L23" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
@@ -1724,7 +1993,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D24">
         <v>4000</v>
@@ -1732,23 +2001,24 @@
       <c r="E24">
         <v>0</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="3">
         <v>4</v>
       </c>
-      <c r="H24">
+      <c r="J24" s="3"/>
+      <c r="K24">
         <v>50</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
       <c r="L24" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.15">
@@ -1759,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D25">
         <v>3000</v>
@@ -1767,23 +2037,23 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="3">
-        <v>5</v>
-      </c>
-      <c r="H25">
-        <v>7</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" s="3">
+        <v>2</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.15">
@@ -1794,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>3000</v>
@@ -1802,23 +2072,23 @@
       <c r="E26">
         <v>0</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="3">
-        <v>5</v>
-      </c>
-      <c r="H26">
-        <v>9</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.15">
@@ -1829,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D27">
         <v>3000</v>
@@ -1837,23 +2107,23 @@
       <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="3">
-        <v>5</v>
-      </c>
-      <c r="H27">
-        <v>11</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="3">
+        <v>2</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
@@ -1864,7 +2134,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D28">
         <v>3000</v>
@@ -1872,23 +2142,23 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="3">
-        <v>5</v>
-      </c>
-      <c r="H28">
-        <v>13</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.15">
@@ -1899,7 +2169,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D29">
         <v>3000</v>
@@ -1907,23 +2177,23 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="3">
-        <v>5</v>
-      </c>
-      <c r="H29">
-        <v>15</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I29" s="3">
+        <v>2</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1936,12 +2206,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="48.625" customWidth="1"/>
+    <col min="4" max="4" width="57.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
rename level -> lv
</commit_message>
<xml_diff>
--- a/plan/excel/aura_光环表.xlsx
+++ b/plan/excel/aura_光环表.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>作者</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -34,7 +34,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -115,7 +115,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>Author:</t>
+          <t>作者:</t>
         </r>
         <r>
           <rPr>
@@ -231,7 +231,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -248,7 +248,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -266,10 +266,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>level</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>number</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -297,7 +293,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -523,7 +519,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -552,7 +548,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -569,7 +565,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -586,7 +582,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -603,7 +599,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -620,7 +616,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -681,7 +677,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -725,16 +721,19 @@
     <t>可否被清除</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>lv</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -761,14 +760,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -819,7 +818,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -835,7 +834,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1125,59 +1124,59 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.75" customWidth="1"/>
-    <col min="8" max="8" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="23.625" customWidth="1"/>
-    <col min="12" max="12" width="37.75" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -1197,101 +1196,101 @@
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="K4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -1299,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>3000</v>
@@ -1314,7 +1313,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -1324,10 +1323,10 @@
         <v>20</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>4000</v>
@@ -1350,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -1360,10 +1359,10 @@
         <v>40</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>2001</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>5000</v>
@@ -1386,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
@@ -1396,10 +1395,10 @@
         <v>60</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>6000</v>
@@ -1422,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
@@ -1432,10 +1431,10 @@
         <v>80</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -1443,7 +1442,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>7000</v>
@@ -1458,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
@@ -1468,10 +1467,10 @@
         <v>100</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -1479,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>4500</v>
@@ -1494,22 +1493,22 @@
         <v>1</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K10">
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>4500</v>
@@ -1532,22 +1531,22 @@
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="3">
         <v>2</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K11">
         <v>20</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12">
         <v>4500</v>
@@ -1570,22 +1569,22 @@
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I12" s="3">
         <v>2</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K12">
         <v>30</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -1593,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>4500</v>
@@ -1608,22 +1607,22 @@
         <v>1</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I13" s="3">
         <v>2</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K13">
         <v>40</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>4500</v>
@@ -1646,22 +1645,22 @@
         <v>1</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I14" s="3">
         <v>2</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K14">
         <v>50</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>2003</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15">
         <v>5000</v>
@@ -1684,20 +1683,20 @@
         <v>1</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I15" s="3">
         <v>3</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>6000</v>
@@ -1720,20 +1719,20 @@
         <v>1</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I16" s="3">
         <v>3</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>2003</v>
       </c>
@@ -1741,7 +1740,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17">
         <v>7000</v>
@@ -1756,20 +1755,20 @@
         <v>1</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" s="3">
         <v>3</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -1777,7 +1776,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>8000</v>
@@ -1792,20 +1791,20 @@
         <v>1</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="3">
         <v>3</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>9000</v>
@@ -1828,20 +1827,20 @@
         <v>1</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="3">
         <v>3</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>2004</v>
       </c>
@@ -1849,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>4000</v>
@@ -1864,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="3">
         <v>4</v>
@@ -1874,10 +1873,10 @@
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>2004</v>
       </c>
@@ -1885,7 +1884,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21">
         <v>4000</v>
@@ -1900,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I21" s="3">
         <v>4</v>
@@ -1910,10 +1909,10 @@
         <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22">
         <v>4000</v>
@@ -1936,7 +1935,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I22" s="3">
         <v>4</v>
@@ -1946,10 +1945,10 @@
         <v>30</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>2004</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <v>4000</v>
@@ -1972,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I23" s="3">
         <v>4</v>
@@ -1982,10 +1981,10 @@
         <v>40</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>2004</v>
       </c>
@@ -1993,7 +1992,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24">
         <v>4000</v>
@@ -2008,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I24" s="3">
         <v>4</v>
@@ -2018,10 +2017,10 @@
         <v>50</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>2005</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25">
         <v>3000</v>
@@ -2044,19 +2043,19 @@
         <v>2</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I25" s="3">
         <v>2</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>2005</v>
       </c>
@@ -2064,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26">
         <v>3000</v>
@@ -2079,19 +2078,19 @@
         <v>2</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I26" s="3">
         <v>2</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>3000</v>
@@ -2114,19 +2113,19 @@
         <v>2</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I27" s="3">
         <v>2</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>2005</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28">
         <v>3000</v>
@@ -2149,19 +2148,19 @@
         <v>2</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I28" s="3">
         <v>2</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>2005</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29">
         <v>3000</v>
@@ -2184,16 +2183,16 @@
         <v>2</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I29" s="3">
         <v>2</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2212,60 +2211,60 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="48.625" customWidth="1"/>
-    <col min="4" max="4" width="57.25" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>